<commit_message>
Changing t test extractor to be slightly broader, building tests for said same
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099FCEE2-DAF1-489C-BB06-FF6CA0C671A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D6BF6F-DF54-49F1-8F8C-1126DB6A29B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2655" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manually_curated_test_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="396">
   <si>
     <t>PMC_ID</t>
   </si>
@@ -1269,6 +1269,15 @@
   </si>
   <si>
     <t>discussion</t>
+  </si>
+  <si>
+    <t>or in self-administration of saccharin-sweetened water (Figures 1c; t(18)=0.83; P=0.42). Note that responding levels for saccharine are equivalent to those for alcohol in the dependent group.</t>
+  </si>
+  <si>
+    <t>The interaction effect between serum cortisol and WMV of the left MTG was not significant (t = 0.698, p = 0.490) after adjusted for the effect of age, years of education and gender.</t>
+  </si>
+  <si>
+    <t>In terms of religious coping, those who belonged to nuclear families (16.11 [5.43] vs. 13.38 [7.17]; t-value 2.083*, [0.040]) and rural locality</t>
   </si>
 </sst>
 </file>
@@ -2133,9 +2142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="86" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P68" sqref="P68"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5505,13 +5514,44 @@
       <c r="C68" t="s">
         <v>210</v>
       </c>
-      <c r="L68" t="e">
-        <f t="shared" ref="L67:L101" ca="1" si="2">RANDBETWEEN(1,K68)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N68" t="e">
-        <f t="shared" ref="N67:N101" ca="1" si="3">RANDBETWEEN(1,M68)</f>
-        <v>#NUM!</v>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" t="s">
+        <v>12</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>4</v>
+      </c>
+      <c r="N68">
+        <v>4</v>
+      </c>
+      <c r="O68" t="s">
+        <v>393</v>
+      </c>
+      <c r="P68" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
@@ -5524,13 +5564,44 @@
       <c r="C69" t="s">
         <v>213</v>
       </c>
-      <c r="L69" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N69" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>80</v>
+      </c>
+      <c r="H69" t="s">
+        <v>12</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69" t="s">
+        <v>12</v>
+      </c>
+      <c r="M69" t="s">
+        <v>12</v>
+      </c>
+      <c r="N69" t="s">
+        <v>12</v>
+      </c>
+      <c r="O69" t="s">
+        <v>12</v>
+      </c>
+      <c r="P69" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
@@ -5543,13 +5614,44 @@
       <c r="C70" t="s">
         <v>216</v>
       </c>
-      <c r="L70" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N70" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>200</v>
+      </c>
+      <c r="H70" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>12</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70" t="s">
+        <v>12</v>
+      </c>
+      <c r="M70" t="s">
+        <v>12</v>
+      </c>
+      <c r="N70" t="s">
+        <v>12</v>
+      </c>
+      <c r="O70" t="s">
+        <v>12</v>
+      </c>
+      <c r="P70" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
@@ -5562,13 +5664,44 @@
       <c r="C71" t="s">
         <v>219</v>
       </c>
-      <c r="L71" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N71" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>41</v>
+      </c>
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>12</v>
+      </c>
+      <c r="K71">
+        <v>5</v>
+      </c>
+      <c r="L71">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+      <c r="O71" t="s">
+        <v>394</v>
+      </c>
+      <c r="P71" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
@@ -5581,13 +5714,44 @@
       <c r="C72" t="s">
         <v>222</v>
       </c>
-      <c r="L72" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N72" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="G72" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" t="s">
+        <v>12</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>12</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72" t="s">
+        <v>12</v>
+      </c>
+      <c r="M72" t="s">
+        <v>12</v>
+      </c>
+      <c r="N72" t="s">
+        <v>12</v>
+      </c>
+      <c r="O72" t="s">
+        <v>12</v>
+      </c>
+      <c r="P72" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
@@ -5600,13 +5764,44 @@
       <c r="C73" t="s">
         <v>225</v>
       </c>
-      <c r="L73" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N73" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s">
+        <v>12</v>
+      </c>
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>12</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73" t="s">
+        <v>12</v>
+      </c>
+      <c r="M73" t="s">
+        <v>12</v>
+      </c>
+      <c r="N73" t="s">
+        <v>12</v>
+      </c>
+      <c r="O73" t="s">
+        <v>12</v>
+      </c>
+      <c r="P73" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
@@ -5619,13 +5814,44 @@
       <c r="C74" t="s">
         <v>228</v>
       </c>
-      <c r="L74" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N74" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>150</v>
+      </c>
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" t="b">
+        <v>0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>12</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>4</v>
+      </c>
+      <c r="N74">
+        <v>3</v>
+      </c>
+      <c r="O74" t="s">
+        <v>395</v>
+      </c>
+      <c r="P74" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
@@ -5638,13 +5864,44 @@
       <c r="C75" t="s">
         <v>231</v>
       </c>
-      <c r="L75" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N75" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>12</v>
+      </c>
+      <c r="H75" t="s">
+        <v>12</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>12</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75" t="s">
+        <v>12</v>
+      </c>
+      <c r="M75" t="s">
+        <v>12</v>
+      </c>
+      <c r="N75" t="s">
+        <v>12</v>
+      </c>
+      <c r="O75" t="s">
+        <v>12</v>
+      </c>
+      <c r="P75" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
@@ -5657,13 +5914,44 @@
       <c r="C76" t="s">
         <v>234</v>
       </c>
-      <c r="L76" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N76" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
+        <v>12</v>
+      </c>
+      <c r="H76" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76" t="b">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>12</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76" t="s">
+        <v>12</v>
+      </c>
+      <c r="M76" t="s">
+        <v>12</v>
+      </c>
+      <c r="N76" t="s">
+        <v>12</v>
+      </c>
+      <c r="O76" t="s">
+        <v>12</v>
+      </c>
+      <c r="P76" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
@@ -5676,12 +5964,15 @@
       <c r="C77" t="s">
         <v>237</v>
       </c>
+      <c r="G77">
+        <v>27</v>
+      </c>
       <c r="L77" t="e">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="L67:L101" ca="1" si="2">RANDBETWEEN(1,K77)</f>
         <v>#NUM!</v>
       </c>
       <c r="N77" t="e">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="N67:N101" ca="1" si="3">RANDBETWEEN(1,M77)</f>
         <v>#NUM!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Makes sure that the "F = 4.96, df = 22, p = 0.001" will be accepted - Closes #54
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D6BF6F-DF54-49F1-8F8C-1126DB6A29B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD562E48-C0AD-4F47-9D9C-07373EE441BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2655" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1680" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manually_curated_test_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="398">
   <si>
     <t>PMC_ID</t>
   </si>
@@ -1278,6 +1278,12 @@
   </si>
   <si>
     <t>In terms of religious coping, those who belonged to nuclear families (16.11 [5.43] vs. 13.38 [7.17]; t-value 2.083*, [0.040]) and rural locality</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At 16 weeks, participants’ weight changed by a mean –3.33 (SD 10.12, range –28.90 to 12.60) pounds from baseline (t26=1.71, P=.09), which is –1.26% of baseline weight (SD 4.55, range –12% to 9%).</t>
   </si>
 </sst>
 </file>
@@ -2142,9 +2148,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="53" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K77" sqref="K77"/>
+      <selection pane="bottomLeft" activeCell="J78" sqref="J78:P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2643,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:N66" ca="1" si="0">RANDBETWEEN(1,M10)</f>
+        <f t="shared" ref="N10" ca="1" si="0">RANDBETWEEN(1,M10)</f>
         <v>1</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -4588,7 +4594,7 @@
         <v>1</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L66" ca="1" si="1">RANDBETWEEN(1,K49)</f>
+        <f t="shared" ref="L49" ca="1" si="1">RANDBETWEEN(1,K49)</f>
         <v>1</v>
       </c>
       <c r="M49">
@@ -5964,16 +5970,44 @@
       <c r="C77" t="s">
         <v>237</v>
       </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
       <c r="G77">
-        <v>27</v>
-      </c>
-      <c r="L77" t="e">
-        <f t="shared" ref="L67:L101" ca="1" si="2">RANDBETWEEN(1,K77)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N77" t="e">
-        <f t="shared" ref="N67:N101" ca="1" si="3">RANDBETWEEN(1,M77)</f>
-        <v>#NUM!</v>
+        <v>47</v>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>12</v>
+      </c>
+      <c r="K77">
+        <v>3</v>
+      </c>
+      <c r="L77">
+        <v>2</v>
+      </c>
+      <c r="M77">
+        <v>3</v>
+      </c>
+      <c r="N77">
+        <v>3</v>
+      </c>
+      <c r="O77" t="s">
+        <v>397</v>
+      </c>
+      <c r="P77" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
@@ -5986,13 +6020,44 @@
       <c r="C78" t="s">
         <v>240</v>
       </c>
-      <c r="L78" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N78" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>11</v>
+      </c>
+      <c r="H78" t="s">
+        <v>12</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>12</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78" t="s">
+        <v>12</v>
+      </c>
+      <c r="M78" t="s">
+        <v>12</v>
+      </c>
+      <c r="N78" t="s">
+        <v>12</v>
+      </c>
+      <c r="O78" t="s">
+        <v>12</v>
+      </c>
+      <c r="P78" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
@@ -6006,11 +6071,11 @@
         <v>243</v>
       </c>
       <c r="L79" t="e">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="L77:L101" ca="1" si="2">RANDBETWEEN(1,K79)</f>
         <v>#NUM!</v>
       </c>
       <c r="N79" t="e">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="N77:N101" ca="1" si="3">RANDBETWEEN(1,M79)</f>
         <v>#NUM!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating manual test set
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD562E48-C0AD-4F47-9D9C-07373EE441BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070FC723-2F9D-4151-AE74-FF46B0E86A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1680" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="3020" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manually_curated_test_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="402">
   <si>
     <t>PMC_ID</t>
   </si>
@@ -1284,6 +1284,18 @@
   </si>
   <si>
     <t xml:space="preserve"> At 16 weeks, participants’ weight changed by a mean –3.33 (SD 10.12, range –28.90 to 12.60) pounds from baseline (t26=1.71, P=.09), which is –1.26% of baseline weight (SD 4.55, range –12% to 9%).</t>
+  </si>
+  <si>
+    <t>The extracted mean volume ± standard deviation of the significant clusters was 4,386 ± 705 mm3 (HEW) and 5,006 ± 693 mm3 (nHEW) in the left hemisphere, with an effect size of 0.89 (Cohen’s d)</t>
+  </si>
+  <si>
+    <t>In the classroom administered reading fluency test (SLS 2-9: Wimmer and Mayringer, 2014; parallel-test reliability r = 0.95 and content validity r = 0.89 for grade 2) children were asked to read sentences silently and to mark them as semantically correct or incorrect (e.g., “Trees can speak”).</t>
+  </si>
+  <si>
+    <t>parallel-test reliability r = 0.95</t>
+  </si>
+  <si>
+    <t>Materials and Methods</t>
   </si>
 </sst>
 </file>
@@ -2148,9 +2160,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="53" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J78" sqref="J78:P78"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6070,13 +6082,44 @@
       <c r="C79" t="s">
         <v>243</v>
       </c>
-      <c r="L79" t="e">
-        <f t="shared" ref="L77:L101" ca="1" si="2">RANDBETWEEN(1,K79)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N79" t="e">
-        <f t="shared" ref="N77:N101" ca="1" si="3">RANDBETWEEN(1,M79)</f>
-        <v>#NUM!</v>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>90</v>
+      </c>
+      <c r="H79" t="s">
+        <v>12</v>
+      </c>
+      <c r="I79" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>12</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79" t="s">
+        <v>12</v>
+      </c>
+      <c r="M79" t="s">
+        <v>12</v>
+      </c>
+      <c r="N79" t="s">
+        <v>12</v>
+      </c>
+      <c r="O79" t="s">
+        <v>12</v>
+      </c>
+      <c r="P79" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
@@ -6089,316 +6132,534 @@
       <c r="C80" t="s">
         <v>246</v>
       </c>
-      <c r="L80" t="e">
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" t="s">
+        <v>12</v>
+      </c>
+      <c r="I80" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>12</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80" t="s">
+        <v>12</v>
+      </c>
+      <c r="M80" t="s">
+        <v>12</v>
+      </c>
+      <c r="N80" t="s">
+        <v>12</v>
+      </c>
+      <c r="O80" t="s">
+        <v>12</v>
+      </c>
+      <c r="P80" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>247</v>
+      </c>
+      <c r="B81" t="s">
+        <v>248</v>
+      </c>
+      <c r="C81" t="s">
+        <v>249</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>66</v>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>12</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
+      <c r="O81" t="s">
+        <v>398</v>
+      </c>
+      <c r="P81" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>250</v>
+      </c>
+      <c r="B82" t="s">
+        <v>251</v>
+      </c>
+      <c r="C82" t="s">
+        <v>252</v>
+      </c>
+      <c r="D82" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+      <c r="G82" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" t="s">
+        <v>12</v>
+      </c>
+      <c r="I82" t="b">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>12</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82" t="s">
+        <v>12</v>
+      </c>
+      <c r="M82" t="s">
+        <v>12</v>
+      </c>
+      <c r="N82" t="s">
+        <v>12</v>
+      </c>
+      <c r="O82" t="s">
+        <v>12</v>
+      </c>
+      <c r="P82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" t="s">
+        <v>255</v>
+      </c>
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>73</v>
+      </c>
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>399</v>
+      </c>
+      <c r="K83">
+        <v>12</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <f t="shared" ref="N77:N101" ca="1" si="2">RANDBETWEEN(1,M83)</f>
+        <v>1</v>
+      </c>
+      <c r="O83" t="s">
+        <v>400</v>
+      </c>
+      <c r="P83" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>256</v>
+      </c>
+      <c r="B84" t="s">
+        <v>257</v>
+      </c>
+      <c r="C84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>7</v>
+      </c>
+      <c r="H84" t="s">
+        <v>12</v>
+      </c>
+      <c r="I84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>12</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84" t="s">
+        <v>12</v>
+      </c>
+      <c r="M84" t="s">
+        <v>12</v>
+      </c>
+      <c r="N84" t="s">
+        <v>12</v>
+      </c>
+      <c r="O84" t="s">
+        <v>12</v>
+      </c>
+      <c r="P84" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C85" t="s">
+        <v>261</v>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>12</v>
+      </c>
+      <c r="H85" t="s">
+        <v>12</v>
+      </c>
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>12</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85" t="s">
+        <v>12</v>
+      </c>
+      <c r="N85" t="s">
+        <v>12</v>
+      </c>
+      <c r="O85" t="s">
+        <v>12</v>
+      </c>
+      <c r="P85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" t="s">
+        <v>264</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" t="s">
+        <v>12</v>
+      </c>
+      <c r="I86" t="b">
+        <v>0</v>
+      </c>
+      <c r="J86" t="s">
+        <v>12</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86" t="s">
+        <v>12</v>
+      </c>
+      <c r="M86" t="s">
+        <v>12</v>
+      </c>
+      <c r="N86" t="s">
+        <v>12</v>
+      </c>
+      <c r="O86" t="s">
+        <v>12</v>
+      </c>
+      <c r="P86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>265</v>
+      </c>
+      <c r="B87" t="s">
+        <v>266</v>
+      </c>
+      <c r="C87" t="s">
+        <v>267</v>
+      </c>
+      <c r="L87" t="e">
+        <f t="shared" ref="L77:L101" ca="1" si="3">RANDBETWEEN(1,K87)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N87" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N80" t="e">
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>268</v>
+      </c>
+      <c r="B88" t="s">
+        <v>269</v>
+      </c>
+      <c r="C88" t="s">
+        <v>270</v>
+      </c>
+      <c r="L88" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>247</v>
-      </c>
-      <c r="B81" t="s">
-        <v>248</v>
-      </c>
-      <c r="C81" t="s">
-        <v>249</v>
-      </c>
-      <c r="L81" t="e">
+      <c r="N88" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N81" t="e">
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>271</v>
+      </c>
+      <c r="B89" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" t="s">
+        <v>273</v>
+      </c>
+      <c r="L89" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>250</v>
-      </c>
-      <c r="B82" t="s">
-        <v>251</v>
-      </c>
-      <c r="C82" t="s">
-        <v>252</v>
-      </c>
-      <c r="L82" t="e">
+      <c r="N89" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N82" t="e">
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>274</v>
+      </c>
+      <c r="B90" t="s">
+        <v>275</v>
+      </c>
+      <c r="C90" t="s">
+        <v>276</v>
+      </c>
+      <c r="L90" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>253</v>
-      </c>
-      <c r="B83" t="s">
-        <v>254</v>
-      </c>
-      <c r="C83" t="s">
-        <v>255</v>
-      </c>
-      <c r="L83" t="e">
+      <c r="N90" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N83" t="e">
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>277</v>
+      </c>
+      <c r="B91" t="s">
+        <v>278</v>
+      </c>
+      <c r="C91" t="s">
+        <v>279</v>
+      </c>
+      <c r="L91" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>256</v>
-      </c>
-      <c r="B84" t="s">
-        <v>257</v>
-      </c>
-      <c r="C84" t="s">
-        <v>258</v>
-      </c>
-      <c r="L84" t="e">
+      <c r="N91" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N84" t="e">
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>280</v>
+      </c>
+      <c r="B92" t="s">
+        <v>281</v>
+      </c>
+      <c r="C92" t="s">
+        <v>282</v>
+      </c>
+      <c r="L92" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>259</v>
-      </c>
-      <c r="B85" t="s">
-        <v>260</v>
-      </c>
-      <c r="C85" t="s">
-        <v>261</v>
-      </c>
-      <c r="L85" t="e">
+      <c r="N92" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N85" t="e">
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>283</v>
+      </c>
+      <c r="B93" t="s">
+        <v>284</v>
+      </c>
+      <c r="C93" t="s">
+        <v>285</v>
+      </c>
+      <c r="L93" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>262</v>
-      </c>
-      <c r="B86" t="s">
-        <v>263</v>
-      </c>
-      <c r="C86" t="s">
-        <v>264</v>
-      </c>
-      <c r="L86" t="e">
+      <c r="N93" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N86" t="e">
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>286</v>
+      </c>
+      <c r="B94" t="s">
+        <v>287</v>
+      </c>
+      <c r="C94" t="s">
+        <v>288</v>
+      </c>
+      <c r="L94" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>265</v>
-      </c>
-      <c r="B87" t="s">
-        <v>266</v>
-      </c>
-      <c r="C87" t="s">
-        <v>267</v>
-      </c>
-      <c r="L87" t="e">
+      <c r="N94" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N87" t="e">
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>289</v>
+      </c>
+      <c r="B95" t="s">
+        <v>290</v>
+      </c>
+      <c r="C95" t="s">
+        <v>291</v>
+      </c>
+      <c r="L95" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>268</v>
-      </c>
-      <c r="B88" t="s">
-        <v>269</v>
-      </c>
-      <c r="C88" t="s">
-        <v>270</v>
-      </c>
-      <c r="L88" t="e">
+      <c r="N95" t="e">
         <f t="shared" ca="1" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="N88" t="e">
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>292</v>
+      </c>
+      <c r="B96" t="s">
+        <v>293</v>
+      </c>
+      <c r="C96" t="s">
+        <v>294</v>
+      </c>
+      <c r="L96" t="e">
         <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>271</v>
-      </c>
-      <c r="B89" t="s">
-        <v>272</v>
-      </c>
-      <c r="C89" t="s">
-        <v>273</v>
-      </c>
-      <c r="L89" t="e">
+      <c r="N96" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N89" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>274</v>
-      </c>
-      <c r="B90" t="s">
-        <v>275</v>
-      </c>
-      <c r="C90" t="s">
-        <v>276</v>
-      </c>
-      <c r="L90" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N90" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>277</v>
-      </c>
-      <c r="B91" t="s">
-        <v>278</v>
-      </c>
-      <c r="C91" t="s">
-        <v>279</v>
-      </c>
-      <c r="L91" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N91" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>280</v>
-      </c>
-      <c r="B92" t="s">
-        <v>281</v>
-      </c>
-      <c r="C92" t="s">
-        <v>282</v>
-      </c>
-      <c r="L92" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N92" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>283</v>
-      </c>
-      <c r="B93" t="s">
-        <v>284</v>
-      </c>
-      <c r="C93" t="s">
-        <v>285</v>
-      </c>
-      <c r="L93" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N93" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>286</v>
-      </c>
-      <c r="B94" t="s">
-        <v>287</v>
-      </c>
-      <c r="C94" t="s">
-        <v>288</v>
-      </c>
-      <c r="L94" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N94" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>289</v>
-      </c>
-      <c r="B95" t="s">
-        <v>290</v>
-      </c>
-      <c r="C95" t="s">
-        <v>291</v>
-      </c>
-      <c r="L95" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N95" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>292</v>
-      </c>
-      <c r="B96" t="s">
-        <v>293</v>
-      </c>
-      <c r="C96" t="s">
-        <v>294</v>
-      </c>
-      <c r="L96" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N96" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6413,11 +6674,11 @@
         <v>297</v>
       </c>
       <c r="L97" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N97" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N97" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6432,11 +6693,11 @@
         <v>300</v>
       </c>
       <c r="L98" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N98" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N98" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6451,11 +6712,11 @@
         <v>303</v>
       </c>
       <c r="L99" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N99" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N99" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6470,11 +6731,11 @@
         <v>306</v>
       </c>
       <c r="L100" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N100" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N100" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -6489,11 +6750,11 @@
         <v>309</v>
       </c>
       <c r="L101" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N101" t="e">
         <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N101" t="e">
-        <f t="shared" ca="1" si="3"/>
         <v>#NUM!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding more to the test set
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070FC723-2F9D-4151-AE74-FF46B0E86A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3C39F9-06A5-4186-A206-E341EEBDDC0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7740" yWindow="3020" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="404">
   <si>
     <t>PMC_ID</t>
   </si>
@@ -1296,6 +1296,12 @@
   </si>
   <si>
     <t>Materials and Methods</t>
+  </si>
+  <si>
+    <t>The Cronbach's alpha for internal consistency reliability was r = 0.76, p &lt; 0.05 suggesting a reasonable reliability.</t>
+  </si>
+  <si>
+    <t>Df 2,218 F = 10.77, p = .000</t>
   </si>
 </sst>
 </file>
@@ -2161,8 +2167,8 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6483,13 +6489,44 @@
       <c r="C87" t="s">
         <v>267</v>
       </c>
-      <c r="L87" t="e">
-        <f t="shared" ref="L77:L101" ca="1" si="3">RANDBETWEEN(1,K87)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N87" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>12</v>
+      </c>
+      <c r="H87" t="s">
+        <v>12</v>
+      </c>
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>12</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87" t="s">
+        <v>12</v>
+      </c>
+      <c r="M87" t="s">
+        <v>12</v>
+      </c>
+      <c r="N87" t="s">
+        <v>12</v>
+      </c>
+      <c r="O87" t="s">
+        <v>12</v>
+      </c>
+      <c r="P87" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.35">
@@ -6502,13 +6539,44 @@
       <c r="C88" t="s">
         <v>270</v>
       </c>
-      <c r="L88" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N88" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>12</v>
+      </c>
+      <c r="H88" t="s">
+        <v>12</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>12</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88" t="s">
+        <v>12</v>
+      </c>
+      <c r="M88" t="s">
+        <v>12</v>
+      </c>
+      <c r="N88" t="s">
+        <v>12</v>
+      </c>
+      <c r="O88" t="s">
+        <v>12</v>
+      </c>
+      <c r="P88" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.35">
@@ -6521,13 +6589,44 @@
       <c r="C89" t="s">
         <v>273</v>
       </c>
-      <c r="L89" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N89" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+      <c r="D89" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s">
+        <v>12</v>
+      </c>
+      <c r="I89" t="b">
+        <v>0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>12</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89" t="s">
+        <v>12</v>
+      </c>
+      <c r="M89" t="s">
+        <v>12</v>
+      </c>
+      <c r="N89" t="s">
+        <v>12</v>
+      </c>
+      <c r="O89" t="s">
+        <v>12</v>
+      </c>
+      <c r="P89" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.35">
@@ -6540,13 +6639,44 @@
       <c r="C90" t="s">
         <v>276</v>
       </c>
-      <c r="L90" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N90" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>139</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" t="s">
+        <v>402</v>
+      </c>
+      <c r="K90">
+        <v>4</v>
+      </c>
+      <c r="L90">
+        <v>2</v>
+      </c>
+      <c r="M90">
+        <v>3</v>
+      </c>
+      <c r="N90">
+        <v>3</v>
+      </c>
+      <c r="O90" t="s">
+        <v>403</v>
+      </c>
+      <c r="P90" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.35">
@@ -6560,7 +6690,7 @@
         <v>279</v>
       </c>
       <c r="L91" t="e">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="L77:L101" ca="1" si="3">RANDBETWEEN(1,K91)</f>
         <v>#NUM!</v>
       </c>
       <c r="N91" t="e">

</xml_diff>

<commit_message>
100 item test set collected
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F81B37B-DAF6-4548-B6C2-6AE98D279914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A421AB2A-C1B1-4B92-A44A-D5F7B6C60AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="3020" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="2328" windowWidth="17280" windowHeight="6228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manually_curated_test_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="410">
   <si>
     <t>PMC_ID</t>
   </si>
@@ -1025,13 +1025,7 @@
     <t>Copy and paste text of the randomly chosen statistical test, include the entire setentence or up until the next or previous statistical test (i.e., do no include any statistical tests apart from the focal analysis)</t>
   </si>
   <si>
-    <t>In addition, the inter-factor correlation values between content factors ranged between 0.22</t>
-  </si>
-  <si>
     <t xml:space="preserve">Significantly more higher educated participants agreed (96%) that 'brisk walking for half an hour most days was good for health' compared to the less educated participants (85%; X2 = 8.08; p = .02). </t>
-  </si>
-  <si>
-    <t>A subsequent regression analysis indicated that the first component (right TPJ, right MFG, and right SPC) correlated significantly with false alarm rates in AVGPs (Figure 4b). Greater activation along this first component corresponded to less false alarms, or better performance, in AVGPs (beta = −0.667, T = −3.35, p = 0.005).</t>
   </si>
   <si>
     <t>test_section</t>
@@ -1308,6 +1302,24 @@
   </si>
   <si>
     <t xml:space="preserve"> and grade point average (F3,223 = 0,672; p = 0,03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similarly, a positive association of L2 proficiency with post-error slowing, r(47) = 0.36, p = 0.006; and post-no-step trials, </t>
+  </si>
+  <si>
+    <t>a significant effect of Block [F (5,80) = 30.46, p &lt; 0.001, Figure 3], and no Block × Treatment interaction</t>
+  </si>
+  <si>
+    <t>η2 = 0.03]. Pairwise comparison showed that patients with DS scored highest, indicating their greatest difficulties, in the VFT P</t>
+  </si>
+  <si>
+    <t>than a single factor model of pain items with depression [χ2 = 126.5 (df = 16, p = 0.0001]; CFI = 0.975; RMSEA = 0.08).</t>
+  </si>
+  <si>
+    <t>and sleep disorders [χ2(3) = 8.03; p = 0.046]. Patients who had waited 6–12 months before HSCT reported higher scores on these scales than did subjects who had waited either less than 6 months or more than 12 months.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Although AVGPs had numerically fewer misses, this difference was not significant t (30)  = −1.348, p = 0.193), and thus all trials were included in the following analyses for both groups.</t>
   </si>
 </sst>
 </file>
@@ -2172,17 +2184,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B102" sqref="A102:XFD116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="10" width="9.1796875" customWidth="1"/>
+    <col min="9" max="10" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2229,10 +2241,10 @@
         <v>326</v>
       </c>
       <c r="P1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2282,7 +2294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2299,7 +2311,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>1027</v>
@@ -2314,25 +2326,25 @@
         <v>324</v>
       </c>
       <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>331</v>
+        <v>12</v>
       </c>
       <c r="P3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2382,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2432,7 +2444,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2476,13 +2488,13 @@
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2514,10 +2526,10 @@
         <v>12</v>
       </c>
       <c r="K7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -2526,13 +2538,13 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>333</v>
+        <v>409</v>
       </c>
       <c r="P7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +2594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2632,7 +2644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2677,13 +2689,13 @@
         <v>1</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2733,7 +2745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2777,13 +2789,13 @@
         <v>2</v>
       </c>
       <c r="O12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2883,7 +2895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2927,13 +2939,13 @@
         <v>1</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2977,13 +2989,13 @@
         <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3027,13 +3039,13 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="P17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -3083,7 +3095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3133,7 +3145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -3183,7 +3195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3197,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -3227,13 +3239,13 @@
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P21" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -3283,7 +3295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -3327,13 +3339,13 @@
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -3362,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -3377,13 +3389,13 @@
         <v>1</v>
       </c>
       <c r="O24" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
@@ -3433,7 +3445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -3483,7 +3495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -3512,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K27">
         <v>13</v>
@@ -3527,13 +3539,13 @@
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P27" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -3577,13 +3589,13 @@
         <v>2</v>
       </c>
       <c r="O28" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="P28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -3633,7 +3645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -3677,13 +3689,13 @@
         <v>3</v>
       </c>
       <c r="O30" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="P30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -3733,7 +3745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>101</v>
       </c>
@@ -3777,13 +3789,13 @@
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="P32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -3827,13 +3839,13 @@
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="P33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -3883,7 +3895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -3933,7 +3945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -3983,7 +3995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -4033,7 +4045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -4083,7 +4095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -4133,7 +4145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -4183,7 +4195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>128</v>
       </c>
@@ -4233,7 +4245,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>131</v>
       </c>
@@ -4277,13 +4289,13 @@
         <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="P42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -4312,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K43">
         <v>2</v>
@@ -4327,13 +4339,13 @@
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="P43" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>137</v>
       </c>
@@ -4377,13 +4389,13 @@
         <v>1</v>
       </c>
       <c r="O44" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="P44" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>140</v>
       </c>
@@ -4427,13 +4439,13 @@
         <v>1</v>
       </c>
       <c r="O45" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="P45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -4483,7 +4495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -4527,13 +4539,13 @@
         <v>1</v>
       </c>
       <c r="O47" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="P47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>148</v>
       </c>
@@ -4577,13 +4589,13 @@
         <v>1</v>
       </c>
       <c r="O48" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P48" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -4612,7 +4624,7 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -4628,13 +4640,13 @@
         <v>5</v>
       </c>
       <c r="O49" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P49" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>154</v>
       </c>
@@ -4684,7 +4696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>157</v>
       </c>
@@ -4713,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K51">
         <v>2</v>
@@ -4728,13 +4740,13 @@
         <v>1</v>
       </c>
       <c r="O51" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="P51" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>160</v>
       </c>
@@ -4763,7 +4775,7 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K52">
         <v>3</v>
@@ -4778,13 +4790,13 @@
         <v>1</v>
       </c>
       <c r="O52" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="P52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -4834,7 +4846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -4878,13 +4890,13 @@
         <v>1</v>
       </c>
       <c r="O54" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="P54" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>169</v>
       </c>
@@ -4928,13 +4940,13 @@
         <v>1</v>
       </c>
       <c r="O55" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="P55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>172</v>
       </c>
@@ -4984,7 +4996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>175</v>
       </c>
@@ -5013,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K57">
         <v>5</v>
@@ -5028,13 +5040,13 @@
         <v>1</v>
       </c>
       <c r="O57" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="P57" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>178</v>
       </c>
@@ -5048,7 +5060,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -5084,7 +5096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>181</v>
       </c>
@@ -5113,7 +5125,7 @@
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -5134,7 +5146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>184</v>
       </c>
@@ -5163,7 +5175,7 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -5184,7 +5196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>187</v>
       </c>
@@ -5213,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K61">
         <v>3</v>
@@ -5228,13 +5240,13 @@
         <v>1</v>
       </c>
       <c r="O61" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="P61" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>190</v>
       </c>
@@ -5263,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -5278,13 +5290,13 @@
         <v>2</v>
       </c>
       <c r="O62" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="P62" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>193</v>
       </c>
@@ -5334,7 +5346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>196</v>
       </c>
@@ -5384,7 +5396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>199</v>
       </c>
@@ -5434,7 +5446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>202</v>
       </c>
@@ -5484,7 +5496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>205</v>
       </c>
@@ -5528,13 +5540,13 @@
         <v>2</v>
       </c>
       <c r="O67" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="P67" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>208</v>
       </c>
@@ -5578,13 +5590,13 @@
         <v>4</v>
       </c>
       <c r="O68" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="P68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>211</v>
       </c>
@@ -5634,7 +5646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>214</v>
       </c>
@@ -5684,7 +5696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>217</v>
       </c>
@@ -5728,13 +5740,13 @@
         <v>1</v>
       </c>
       <c r="O71" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="P71" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>220</v>
       </c>
@@ -5784,7 +5796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>223</v>
       </c>
@@ -5834,7 +5846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>226</v>
       </c>
@@ -5878,13 +5890,13 @@
         <v>3</v>
       </c>
       <c r="O74" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="P74" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>229</v>
       </c>
@@ -5934,7 +5946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>232</v>
       </c>
@@ -5984,7 +5996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>235</v>
       </c>
@@ -6028,13 +6040,13 @@
         <v>3</v>
       </c>
       <c r="O77" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="P77" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>238</v>
       </c>
@@ -6084,7 +6096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>241</v>
       </c>
@@ -6134,7 +6146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>244</v>
       </c>
@@ -6184,7 +6196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>247</v>
       </c>
@@ -6228,13 +6240,13 @@
         <v>1</v>
       </c>
       <c r="O81" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P81" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>250</v>
       </c>
@@ -6284,7 +6296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>253</v>
       </c>
@@ -6313,29 +6325,29 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
+        <v>397</v>
+      </c>
+      <c r="K83">
+        <v>12</v>
+      </c>
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <f t="shared" ref="N83" ca="1" si="2">RANDBETWEEN(1,M83)</f>
+        <v>1</v>
+      </c>
+      <c r="O83" t="s">
+        <v>398</v>
+      </c>
+      <c r="P83" t="s">
         <v>399</v>
       </c>
-      <c r="K83">
-        <v>12</v>
-      </c>
-      <c r="L83">
-        <v>1</v>
-      </c>
-      <c r="M83">
-        <v>1</v>
-      </c>
-      <c r="N83">
-        <f t="shared" ref="N77:N101" ca="1" si="2">RANDBETWEEN(1,M83)</f>
-        <v>1</v>
-      </c>
-      <c r="O83" t="s">
-        <v>400</v>
-      </c>
-      <c r="P83" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>256</v>
       </c>
@@ -6385,7 +6397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>259</v>
       </c>
@@ -6435,7 +6447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>262</v>
       </c>
@@ -6485,7 +6497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>265</v>
       </c>
@@ -6535,7 +6547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>268</v>
       </c>
@@ -6585,7 +6597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -6635,7 +6647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -6664,7 +6676,7 @@
         <v>1</v>
       </c>
       <c r="J90" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K90">
         <v>4</v>
@@ -6679,13 +6691,13 @@
         <v>3</v>
       </c>
       <c r="O90" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="P90" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -6735,7 +6747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -6785,7 +6797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -6835,7 +6847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -6864,7 +6876,7 @@
         <v>1</v>
       </c>
       <c r="J94" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K94">
         <v>2</v>
@@ -6879,13 +6891,13 @@
         <v>8</v>
       </c>
       <c r="O94" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="P94" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>289</v>
       </c>
@@ -6895,16 +6907,47 @@
       <c r="C95" t="s">
         <v>291</v>
       </c>
-      <c r="L95" t="e">
-        <f t="shared" ref="L77:L101" ca="1" si="3">RANDBETWEEN(1,K95)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N95" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>47</v>
+      </c>
+      <c r="H95" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" t="b">
+        <v>0</v>
+      </c>
+      <c r="J95" t="s">
+        <v>12</v>
+      </c>
+      <c r="K95">
+        <v>13</v>
+      </c>
+      <c r="L95">
+        <v>6</v>
+      </c>
+      <c r="M95">
+        <v>3</v>
+      </c>
+      <c r="N95">
+        <v>2</v>
+      </c>
+      <c r="O95" t="s">
+        <v>404</v>
+      </c>
+      <c r="P95" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>292</v>
       </c>
@@ -6914,16 +6957,47 @@
       <c r="C96" t="s">
         <v>294</v>
       </c>
-      <c r="L96" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N96" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>18</v>
+      </c>
+      <c r="H96" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" t="b">
+        <v>0</v>
+      </c>
+      <c r="J96" t="s">
+        <v>12</v>
+      </c>
+      <c r="K96">
+        <v>2</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <v>3</v>
+      </c>
+      <c r="N96">
+        <v>2</v>
+      </c>
+      <c r="O96" t="s">
+        <v>405</v>
+      </c>
+      <c r="P96" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>295</v>
       </c>
@@ -6933,16 +7007,47 @@
       <c r="C97" t="s">
         <v>297</v>
       </c>
-      <c r="L97" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N97" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>148</v>
+      </c>
+      <c r="H97" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" t="s">
+        <v>12</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>6</v>
+      </c>
+      <c r="N97">
+        <v>6</v>
+      </c>
+      <c r="O97" t="s">
+        <v>406</v>
+      </c>
+      <c r="P97" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>298</v>
       </c>
@@ -6952,16 +7057,47 @@
       <c r="C98" t="s">
         <v>300</v>
       </c>
-      <c r="L98" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N98" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" t="s">
+        <v>12</v>
+      </c>
+      <c r="I98" t="s">
+        <v>12</v>
+      </c>
+      <c r="J98" t="s">
+        <v>12</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98" t="s">
+        <v>12</v>
+      </c>
+      <c r="M98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N98" t="s">
+        <v>12</v>
+      </c>
+      <c r="O98" t="s">
+        <v>12</v>
+      </c>
+      <c r="P98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>301</v>
       </c>
@@ -6971,16 +7107,47 @@
       <c r="C99" t="s">
         <v>303</v>
       </c>
-      <c r="L99" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N99" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>12</v>
+      </c>
+      <c r="H99" t="s">
+        <v>12</v>
+      </c>
+      <c r="I99" t="s">
+        <v>12</v>
+      </c>
+      <c r="J99" t="s">
+        <v>12</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99" t="s">
+        <v>12</v>
+      </c>
+      <c r="M99" t="s">
+        <v>12</v>
+      </c>
+      <c r="N99" t="s">
+        <v>12</v>
+      </c>
+      <c r="O99" t="s">
+        <v>12</v>
+      </c>
+      <c r="P99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -6990,16 +7157,47 @@
       <c r="C100" t="s">
         <v>306</v>
       </c>
-      <c r="L100" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N100" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>1078</v>
+      </c>
+      <c r="H100" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" t="s">
+        <v>12</v>
+      </c>
+      <c r="J100" t="s">
+        <v>12</v>
+      </c>
+      <c r="K100">
+        <v>3</v>
+      </c>
+      <c r="L100">
+        <v>3</v>
+      </c>
+      <c r="M100">
+        <v>2</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+      <c r="O100" t="s">
+        <v>407</v>
+      </c>
+      <c r="P100" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -7009,13 +7207,44 @@
       <c r="C101" t="s">
         <v>309</v>
       </c>
-      <c r="L101" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N101" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NUM!</v>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>21</v>
+      </c>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="b">
+        <v>0</v>
+      </c>
+      <c r="J101" t="s">
+        <v>12</v>
+      </c>
+      <c r="K101">
+        <v>5</v>
+      </c>
+      <c r="L101">
+        <v>4</v>
+      </c>
+      <c r="M101">
+        <v>5</v>
+      </c>
+      <c r="N101">
+        <v>5</v>
+      </c>
+      <c r="O101" t="s">
+        <v>408</v>
+      </c>
+      <c r="P101" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -7032,9 +7261,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>314</v>
       </c>
@@ -7042,7 +7271,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7050,7 +7279,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -7058,7 +7287,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -7066,7 +7295,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -7074,15 +7303,15 @@
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -7090,7 +7319,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>320</v>
       </c>
@@ -7098,15 +7327,15 @@
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>313</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -7114,15 +7343,15 @@
         <v>319</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>311</v>
       </c>
       <c r="B11" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -7130,7 +7359,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>326</v>
       </c>
@@ -7151,39 +7380,39 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>368</v>
-      </c>
       <c r="B6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup of old manually extracted xlsx file
</commit_message>
<xml_diff>
--- a/tests/testthat/manually_curated_test_set.xlsx
+++ b/tests/testthat/manually_curated_test_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\EffectSizeScrapingPaper\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850989ED-D2E4-48CA-AB79-6863D4BADF63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76E54C6-25FB-4DA9-8D9F-58BBFFE0842D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="2700" windowWidth="17280" windowHeight="6228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manually_curated_test_set" sheetId="1" r:id="rId1"/>
@@ -2253,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>

</xml_diff>